<commit_message>
Large improvement to geotools and other bug fixes.
</commit_message>
<xml_diff>
--- a/data/country-codes.xlsx
+++ b/data/country-codes.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4241" uniqueCount="2517">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4245" uniqueCount="2520">
   <si>
     <t>GAUL</t>
   </si>
@@ -7449,9 +7449,6 @@
     <t>United States</t>
   </si>
   <si>
-    <t>otherCountryNames</t>
-  </si>
-  <si>
     <t>America</t>
   </si>
   <si>
@@ -7570,6 +7567,18 @@
   </si>
   <si>
     <t>FX</t>
+  </si>
+  <si>
+    <t>otherNames</t>
+  </si>
+  <si>
+    <t>Zaire|Kinshasa</t>
+  </si>
+  <si>
+    <t>Burma</t>
+  </si>
+  <si>
+    <t>Comoros Islands</t>
   </si>
 </sst>
 </file>
@@ -8383,10 +8392,10 @@
   <dimension ref="A1:V266"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B248" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B47" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D257" sqref="D257"/>
+      <selection pane="bottomRight" activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8415,7 +8424,7 @@
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>2503</v>
+        <v>2502</v>
       </c>
       <c r="B1" t="s">
         <v>2443</v>
@@ -8424,10 +8433,10 @@
         <v>2444</v>
       </c>
       <c r="D1" t="s">
-        <v>2476</v>
+        <v>2516</v>
       </c>
       <c r="E1" t="s">
-        <v>2504</v>
+        <v>2503</v>
       </c>
       <c r="F1" t="s">
         <v>2445</v>
@@ -8492,7 +8501,7 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F2" t="s">
         <v>2</v>
@@ -8557,7 +8566,7 @@
         <v>13</v>
       </c>
       <c r="E3" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F3" t="s">
         <v>14</v>
@@ -8622,7 +8631,7 @@
         <v>24</v>
       </c>
       <c r="E4" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F4" t="s">
         <v>25</v>
@@ -8687,7 +8696,7 @@
         <v>36</v>
       </c>
       <c r="E5" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F5" t="s">
         <v>9</v>
@@ -8752,7 +8761,7 @@
         <v>51</v>
       </c>
       <c r="E6" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F6" t="s">
         <v>52</v>
@@ -8817,7 +8826,7 @@
         <v>61</v>
       </c>
       <c r="E7" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F7" t="s">
         <v>62</v>
@@ -8882,7 +8891,7 @@
         <v>71</v>
       </c>
       <c r="E8" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F8" t="s">
         <v>72</v>
@@ -8944,7 +8953,7 @@
         <v>84</v>
       </c>
       <c r="E9" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F9" t="s">
         <v>41</v>
@@ -8988,7 +8997,7 @@
         <v>93</v>
       </c>
       <c r="E10" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F10" t="s">
         <v>28</v>
@@ -9053,7 +9062,7 @@
         <v>104</v>
       </c>
       <c r="E11" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F11" t="s">
         <v>105</v>
@@ -9118,7 +9127,7 @@
         <v>115</v>
       </c>
       <c r="E12" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F12" t="s">
         <v>116</v>
@@ -9183,7 +9192,7 @@
         <v>124</v>
       </c>
       <c r="E13" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F13" t="s">
         <v>125</v>
@@ -9248,7 +9257,7 @@
         <v>137</v>
       </c>
       <c r="E14" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F14" t="s">
         <v>138</v>
@@ -9313,7 +9322,7 @@
         <v>147</v>
       </c>
       <c r="E15" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F15" t="s">
         <v>95</v>
@@ -9378,7 +9387,7 @@
         <v>154</v>
       </c>
       <c r="E16" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F16" t="s">
         <v>155</v>
@@ -9443,7 +9452,7 @@
         <v>164</v>
       </c>
       <c r="E17" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F17" t="s">
         <v>165</v>
@@ -9508,7 +9517,7 @@
         <v>178</v>
       </c>
       <c r="E18" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F18" t="s">
         <v>179</v>
@@ -9573,7 +9582,7 @@
         <v>189</v>
       </c>
       <c r="E19" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F19" t="s">
         <v>190</v>
@@ -9638,7 +9647,7 @@
         <v>202</v>
       </c>
       <c r="E20" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F20" t="s">
         <v>203</v>
@@ -9703,7 +9712,7 @@
         <v>215</v>
       </c>
       <c r="E21" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F21" t="s">
         <v>216</v>
@@ -9768,7 +9777,7 @@
         <v>226</v>
       </c>
       <c r="E22" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F22" t="s">
         <v>227</v>
@@ -9833,7 +9842,7 @@
         <v>234</v>
       </c>
       <c r="E23" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F23" t="s">
         <v>235</v>
@@ -9898,7 +9907,7 @@
         <v>245</v>
       </c>
       <c r="E24" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F24" t="s">
         <v>246</v>
@@ -9963,7 +9972,7 @@
         <v>255</v>
       </c>
       <c r="E25" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F25" t="s">
         <v>256</v>
@@ -10028,7 +10037,7 @@
         <v>267</v>
       </c>
       <c r="E26" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F26" t="s">
         <v>268</v>
@@ -10093,7 +10102,7 @@
         <v>279</v>
       </c>
       <c r="E27" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F27" t="s">
         <v>218</v>
@@ -10158,7 +10167,7 @@
         <v>290</v>
       </c>
       <c r="E28" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F28" t="s">
         <v>168</v>
@@ -10223,7 +10232,7 @@
         <v>299</v>
       </c>
       <c r="E29" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F29" t="s">
         <v>192</v>
@@ -10282,7 +10291,7 @@
         <v>309</v>
       </c>
       <c r="E30" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F30" t="s">
         <v>310</v>
@@ -10323,7 +10332,7 @@
         <v>315</v>
       </c>
       <c r="E31" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F31" t="s">
         <v>205</v>
@@ -10382,7 +10391,7 @@
         <v>323</v>
       </c>
       <c r="E32" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F32" t="s">
         <v>324</v>
@@ -10429,7 +10438,7 @@
         <v>330</v>
       </c>
       <c r="E33" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F33" t="s">
         <v>331</v>
@@ -10494,7 +10503,7 @@
         <v>342</v>
       </c>
       <c r="E34" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F34" t="s">
         <v>181</v>
@@ -10559,7 +10568,7 @@
         <v>351</v>
       </c>
       <c r="E35" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F35" t="s">
         <v>194</v>
@@ -10624,7 +10633,7 @@
         <v>361</v>
       </c>
       <c r="E36" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F36" t="s">
         <v>170</v>
@@ -10689,7 +10698,7 @@
         <v>369</v>
       </c>
       <c r="E37" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F37" t="s">
         <v>370</v>
@@ -10754,7 +10763,7 @@
         <v>380</v>
       </c>
       <c r="E38" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F38" t="s">
         <v>381</v>
@@ -10819,7 +10828,7 @@
         <v>393</v>
       </c>
       <c r="E39" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F39" t="s">
         <v>394</v>
@@ -10884,7 +10893,7 @@
         <v>402</v>
       </c>
       <c r="E40" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F40" t="s">
         <v>403</v>
@@ -10949,7 +10958,7 @@
         <v>413</v>
       </c>
       <c r="E41" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F41" t="s">
         <v>414</v>
@@ -11014,7 +11023,7 @@
         <v>424</v>
       </c>
       <c r="E42" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F42" t="s">
         <v>425</v>
@@ -11076,7 +11085,7 @@
         <v>433</v>
       </c>
       <c r="E43" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F43" t="s">
         <v>434</v>
@@ -11141,7 +11150,7 @@
         <v>446</v>
       </c>
       <c r="E44" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F44" t="s">
         <v>447</v>
@@ -11206,7 +11215,7 @@
         <v>457</v>
       </c>
       <c r="E45" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F45" t="s">
         <v>458</v>
@@ -11271,7 +11280,7 @@
         <v>467</v>
       </c>
       <c r="E46" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F46" t="s">
         <v>468</v>
@@ -11336,7 +11345,7 @@
         <v>480</v>
       </c>
       <c r="E47" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F47" t="s">
         <v>405</v>
@@ -11395,7 +11404,7 @@
         <v>488</v>
       </c>
       <c r="E48" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F48" t="s">
         <v>489</v>
@@ -11439,7 +11448,7 @@
         <v>497</v>
       </c>
       <c r="E49" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F49" t="s">
         <v>498</v>
@@ -11489,7 +11498,7 @@
         <v>505</v>
       </c>
       <c r="E50" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F50" t="s">
         <v>506</v>
@@ -11553,8 +11562,11 @@
       <c r="C51" t="s">
         <v>515</v>
       </c>
+      <c r="D51" t="s">
+        <v>2519</v>
+      </c>
       <c r="E51" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F51" t="s">
         <v>516</v>
@@ -11618,8 +11630,11 @@
       <c r="C52" t="s">
         <v>526</v>
       </c>
+      <c r="D52" t="s">
+        <v>531</v>
+      </c>
       <c r="E52" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F52" t="s">
         <v>527</v>
@@ -11683,8 +11698,11 @@
       <c r="C53" t="s">
         <v>536</v>
       </c>
+      <c r="D53" t="s">
+        <v>2517</v>
+      </c>
       <c r="E53" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F53" t="s">
         <v>460</v>
@@ -11737,7 +11755,7 @@
         <v>542</v>
       </c>
       <c r="E54" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F54" t="s">
         <v>500</v>
@@ -11802,7 +11820,7 @@
         <v>554</v>
       </c>
       <c r="E55" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F55" t="s">
         <v>555</v>
@@ -11867,7 +11885,7 @@
         <v>565</v>
       </c>
       <c r="E56" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F56" t="s">
         <v>566</v>
@@ -11932,7 +11950,7 @@
         <v>575</v>
       </c>
       <c r="E57" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F57" t="s">
         <v>576</v>
@@ -11997,7 +12015,7 @@
         <v>584</v>
       </c>
       <c r="E58" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F58" t="s">
         <v>546</v>
@@ -12053,7 +12071,7 @@
         <v>593</v>
       </c>
       <c r="E59" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F59" t="s">
         <v>594</v>
@@ -12118,7 +12136,7 @@
         <v>602</v>
       </c>
       <c r="E60" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F60" t="s">
         <v>603</v>
@@ -12171,7 +12189,7 @@
         <v>610</v>
       </c>
       <c r="E61" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F61" t="s">
         <v>472</v>
@@ -12236,7 +12254,7 @@
         <v>618</v>
       </c>
       <c r="E62" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F62" t="s">
         <v>619</v>
@@ -12301,7 +12319,7 @@
         <v>629</v>
       </c>
       <c r="E63" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F63" t="s">
         <v>630</v>
@@ -12366,7 +12384,7 @@
         <v>638</v>
       </c>
       <c r="E64" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F64" t="s">
         <v>639</v>
@@ -12431,7 +12449,7 @@
         <v>648</v>
       </c>
       <c r="E65" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F65" t="s">
         <v>641</v>
@@ -12496,7 +12514,7 @@
         <v>659</v>
       </c>
       <c r="E66" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F66" t="s">
         <v>660</v>
@@ -12561,7 +12579,7 @@
         <v>667</v>
       </c>
       <c r="E67" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F67" t="s">
         <v>668</v>
@@ -12626,7 +12644,7 @@
         <v>677</v>
       </c>
       <c r="E68" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F68" t="s">
         <v>678</v>
@@ -12691,7 +12709,7 @@
         <v>687</v>
       </c>
       <c r="E69" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F69" t="s">
         <v>688</v>
@@ -12756,7 +12774,7 @@
         <v>698</v>
       </c>
       <c r="E70" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F70" t="s">
         <v>699</v>
@@ -12821,7 +12839,7 @@
         <v>708</v>
       </c>
       <c r="E71" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F71" t="s">
         <v>709</v>
@@ -12886,7 +12904,7 @@
         <v>717</v>
       </c>
       <c r="E72" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F72" t="s">
         <v>670</v>
@@ -12951,7 +12969,7 @@
         <v>727</v>
       </c>
       <c r="E73" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F73" t="s">
         <v>728</v>
@@ -13016,7 +13034,7 @@
         <v>738</v>
       </c>
       <c r="E74" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F74" t="s">
         <v>739</v>
@@ -13069,7 +13087,7 @@
         <v>747</v>
       </c>
       <c r="E75" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F75" t="s">
         <v>748</v>
@@ -13134,7 +13152,7 @@
         <v>758</v>
       </c>
       <c r="E76" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F76" t="s">
         <v>759</v>
@@ -13199,7 +13217,7 @@
         <v>765</v>
       </c>
       <c r="E77" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F77" t="s">
         <v>766</v>
@@ -13264,7 +13282,7 @@
         <v>774</v>
       </c>
       <c r="E78" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F78" t="s">
         <v>775</v>
@@ -13329,7 +13347,7 @@
         <v>785</v>
       </c>
       <c r="E79" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F79" t="s">
         <v>786</v>
@@ -13388,7 +13406,7 @@
         <v>798</v>
       </c>
       <c r="E80" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F80" t="s">
         <v>799</v>
@@ -13435,7 +13453,7 @@
         <v>804</v>
       </c>
       <c r="E81" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F81" t="s">
         <v>805</v>
@@ -13500,7 +13518,7 @@
         <v>813</v>
       </c>
       <c r="E82" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F82" t="s">
         <v>814</v>
@@ -13565,7 +13583,7 @@
         <v>824</v>
       </c>
       <c r="E83" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F83" t="s">
         <v>825</v>
@@ -13630,7 +13648,7 @@
         <v>835</v>
       </c>
       <c r="E84" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F84" t="s">
         <v>836</v>
@@ -13695,7 +13713,7 @@
         <v>843</v>
       </c>
       <c r="E85" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F85" t="s">
         <v>844</v>
@@ -13760,7 +13778,7 @@
         <v>852</v>
       </c>
       <c r="E86" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F86" t="s">
         <v>853</v>
@@ -13825,7 +13843,7 @@
         <v>862</v>
       </c>
       <c r="E87" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F87" t="s">
         <v>863</v>
@@ -13890,7 +13908,7 @@
         <v>871</v>
       </c>
       <c r="E88" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F88" t="s">
         <v>872</v>
@@ -13955,7 +13973,7 @@
         <v>879</v>
       </c>
       <c r="E89" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F89" t="s">
         <v>880</v>
@@ -14020,7 +14038,7 @@
         <v>889</v>
       </c>
       <c r="E90" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F90" t="s">
         <v>890</v>
@@ -14085,7 +14103,7 @@
         <v>898</v>
       </c>
       <c r="E91" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F91" t="s">
         <v>899</v>
@@ -14150,7 +14168,7 @@
         <v>906</v>
       </c>
       <c r="E92" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F92" t="s">
         <v>907</v>
@@ -14215,7 +14233,7 @@
         <v>917</v>
       </c>
       <c r="E93" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F93" t="s">
         <v>827</v>
@@ -14277,7 +14295,7 @@
         <v>929</v>
       </c>
       <c r="E94" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F94" t="s">
         <v>930</v>
@@ -14342,7 +14360,7 @@
         <v>941</v>
       </c>
       <c r="E95" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F95" t="s">
         <v>942</v>
@@ -14407,7 +14425,7 @@
         <v>950</v>
       </c>
       <c r="E96" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F96" t="s">
         <v>951</v>
@@ -14472,7 +14490,7 @@
         <v>960</v>
       </c>
       <c r="E97" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F97" t="s">
         <v>961</v>
@@ -14531,7 +14549,7 @@
         <v>969</v>
       </c>
       <c r="E98" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F98" t="s">
         <v>970</v>
@@ -14572,7 +14590,7 @@
         <v>973</v>
       </c>
       <c r="E99" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F99" t="s">
         <v>974</v>
@@ -14637,7 +14655,7 @@
         <v>986</v>
       </c>
       <c r="E100" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F100" t="s">
         <v>987</v>
@@ -14690,7 +14708,7 @@
         <v>993</v>
       </c>
       <c r="E101" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F101" t="s">
         <v>994</v>
@@ -14755,7 +14773,7 @@
         <v>1003</v>
       </c>
       <c r="E102" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F102" t="s">
         <v>1004</v>
@@ -14820,7 +14838,7 @@
         <v>1014</v>
       </c>
       <c r="E103" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F103" t="s">
         <v>1015</v>
@@ -14885,7 +14903,7 @@
         <v>1022</v>
       </c>
       <c r="E104" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F104" t="s">
         <v>1023</v>
@@ -14950,7 +14968,7 @@
         <v>1034</v>
       </c>
       <c r="E105" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F105" t="s">
         <v>1035</v>
@@ -15015,7 +15033,7 @@
         <v>1044</v>
       </c>
       <c r="E106" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F106" t="s">
         <v>1045</v>
@@ -15080,7 +15098,7 @@
         <v>1055</v>
       </c>
       <c r="E107" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F107" t="s">
         <v>1056</v>
@@ -15145,7 +15163,7 @@
         <v>1064</v>
       </c>
       <c r="E108" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F108" t="s">
         <v>1065</v>
@@ -15207,7 +15225,7 @@
         <v>1073</v>
       </c>
       <c r="E109" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F109" t="s">
         <v>1006</v>
@@ -15272,7 +15290,7 @@
         <v>1082</v>
       </c>
       <c r="E110" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F110" t="s">
         <v>1083</v>
@@ -15337,7 +15355,7 @@
         <v>1090</v>
       </c>
       <c r="E111" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F111" t="s">
         <v>1091</v>
@@ -15402,7 +15420,7 @@
         <v>1102</v>
       </c>
       <c r="E112" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F112" t="s">
         <v>1103</v>
@@ -15467,7 +15485,7 @@
         <v>1111</v>
       </c>
       <c r="E113" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F113" t="s">
         <v>1112</v>
@@ -15529,7 +15547,7 @@
         <v>1120</v>
       </c>
       <c r="E114" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F114" t="s">
         <v>1121</v>
@@ -15594,7 +15612,7 @@
         <v>1129</v>
       </c>
       <c r="E115" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F115" t="s">
         <v>1130</v>
@@ -15659,7 +15677,7 @@
         <v>1138</v>
       </c>
       <c r="E116" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F116" t="s">
         <v>1139</v>
@@ -15724,7 +15742,7 @@
         <v>1148</v>
       </c>
       <c r="E117" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F117" t="s">
         <v>491</v>
@@ -15789,7 +15807,7 @@
         <v>1156</v>
       </c>
       <c r="E118" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F118" t="s">
         <v>1157</v>
@@ -15854,7 +15872,7 @@
         <v>1167</v>
       </c>
       <c r="E119" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F119" t="s">
         <v>1168</v>
@@ -15919,7 +15937,7 @@
         <v>1179</v>
       </c>
       <c r="E120" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F120" t="s">
         <v>1180</v>
@@ -15984,7 +16002,7 @@
         <v>1189</v>
       </c>
       <c r="E121" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F121" t="s">
         <v>1190</v>
@@ -16049,7 +16067,7 @@
         <v>1199</v>
       </c>
       <c r="E122" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F122" t="s">
         <v>1200</v>
@@ -16114,7 +16132,7 @@
         <v>1210</v>
       </c>
       <c r="E123" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F123" t="s">
         <v>1211</v>
@@ -16179,7 +16197,7 @@
         <v>1222</v>
       </c>
       <c r="E124" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F124" t="s">
         <v>1223</v>
@@ -16244,7 +16262,7 @@
         <v>1233</v>
       </c>
       <c r="E125" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F125" t="s">
         <v>1234</v>
@@ -16309,7 +16327,7 @@
         <v>1243</v>
       </c>
       <c r="E126" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F126" t="s">
         <v>1225</v>
@@ -16374,7 +16392,7 @@
         <v>1252</v>
       </c>
       <c r="E127" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F127" t="s">
         <v>1214</v>
@@ -16439,7 +16457,7 @@
         <v>1259</v>
       </c>
       <c r="E128" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F128" t="s">
         <v>1260</v>
@@ -16504,7 +16522,7 @@
         <v>1267</v>
       </c>
       <c r="E129" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F129" t="s">
         <v>1268</v>
@@ -16569,7 +16587,7 @@
         <v>1280</v>
       </c>
       <c r="E130" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F130" t="s">
         <v>1281</v>
@@ -16634,7 +16652,7 @@
         <v>1289</v>
       </c>
       <c r="E131" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F131" t="s">
         <v>1290</v>
@@ -16699,7 +16717,7 @@
         <v>1301</v>
       </c>
       <c r="E132" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F132" t="s">
         <v>1302</v>
@@ -16764,7 +16782,7 @@
         <v>1313</v>
       </c>
       <c r="E133" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F133" t="s">
         <v>1314</v>
@@ -16829,7 +16847,7 @@
         <v>1325</v>
       </c>
       <c r="E134" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F134" t="s">
         <v>1326</v>
@@ -16894,7 +16912,7 @@
         <v>1334</v>
       </c>
       <c r="E135" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F135" t="s">
         <v>1335</v>
@@ -16959,7 +16977,7 @@
         <v>1342</v>
       </c>
       <c r="E136" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F136" t="s">
         <v>1343</v>
@@ -17024,7 +17042,7 @@
         <v>1350</v>
       </c>
       <c r="E137" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F137" t="s">
         <v>1351</v>
@@ -17089,7 +17107,7 @@
         <v>1358</v>
       </c>
       <c r="E138" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F138" t="s">
         <v>1359</v>
@@ -17154,7 +17172,7 @@
         <v>1369</v>
       </c>
       <c r="E139" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F139" t="s">
         <v>1362</v>
@@ -17219,7 +17237,7 @@
         <v>1378</v>
       </c>
       <c r="E140" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F140" t="s">
         <v>1270</v>
@@ -17284,7 +17302,7 @@
         <v>1388</v>
       </c>
       <c r="E141" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F141" t="s">
         <v>1389</v>
@@ -17349,7 +17367,7 @@
         <v>1397</v>
       </c>
       <c r="E142" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F142" t="s">
         <v>1398</v>
@@ -17414,7 +17432,7 @@
         <v>1408</v>
       </c>
       <c r="E143" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F143" t="s">
         <v>1409</v>
@@ -17479,7 +17497,7 @@
         <v>1417</v>
       </c>
       <c r="E144" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F144" t="s">
         <v>1418</v>
@@ -17544,7 +17562,7 @@
         <v>1426</v>
       </c>
       <c r="E145" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F145" t="s">
         <v>1271</v>
@@ -17609,7 +17627,7 @@
         <v>1434</v>
       </c>
       <c r="E146" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F146" t="s">
         <v>1429</v>
@@ -17674,7 +17692,7 @@
         <v>1444</v>
       </c>
       <c r="E147" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F147" t="s">
         <v>1445</v>
@@ -17739,7 +17757,7 @@
         <v>1452</v>
       </c>
       <c r="E148" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F148" t="s">
         <v>1317</v>
@@ -17804,7 +17822,7 @@
         <v>1460</v>
       </c>
       <c r="E149" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F149" t="s">
         <v>1294</v>
@@ -17869,7 +17887,7 @@
         <v>1467</v>
       </c>
       <c r="E150" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F150" t="s">
         <v>1468</v>
@@ -17933,8 +17951,11 @@
       <c r="C151" t="s">
         <v>1476</v>
       </c>
+      <c r="D151" t="s">
+        <v>2518</v>
+      </c>
       <c r="E151" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F151" t="s">
         <v>1477</v>
@@ -17999,7 +18020,7 @@
         <v>1486</v>
       </c>
       <c r="E152" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F152" t="s">
         <v>81</v>
@@ -18064,7 +18085,7 @@
         <v>1493</v>
       </c>
       <c r="E153" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F153" t="s">
         <v>1494</v>
@@ -18129,7 +18150,7 @@
         <v>1502</v>
       </c>
       <c r="E154" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F154" t="s">
         <v>1503</v>
@@ -18194,7 +18215,7 @@
         <v>1513</v>
       </c>
       <c r="E155" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F155" t="s">
         <v>427</v>
@@ -18259,7 +18280,7 @@
         <v>1521</v>
       </c>
       <c r="E156" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F156" t="s">
         <v>1522</v>
@@ -18324,7 +18345,7 @@
         <v>1530</v>
       </c>
       <c r="E157" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F157" t="s">
         <v>545</v>
@@ -18389,7 +18410,7 @@
         <v>1536</v>
       </c>
       <c r="E158" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F158" t="s">
         <v>1537</v>
@@ -18454,7 +18475,7 @@
         <v>1546</v>
       </c>
       <c r="E159" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F159" t="s">
         <v>1547</v>
@@ -18519,7 +18540,7 @@
         <v>1558</v>
       </c>
       <c r="E160" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F160" t="s">
         <v>1552</v>
@@ -18584,7 +18605,7 @@
         <v>1567</v>
       </c>
       <c r="E161" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F161" t="s">
         <v>127</v>
@@ -18649,7 +18670,7 @@
         <v>1574</v>
       </c>
       <c r="E162" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F162" t="s">
         <v>1575</v>
@@ -18714,7 +18735,7 @@
         <v>1583</v>
       </c>
       <c r="E163" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F163" t="s">
         <v>383</v>
@@ -18779,7 +18800,7 @@
         <v>1592</v>
       </c>
       <c r="E164" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F164" t="s">
         <v>1381</v>
@@ -18844,7 +18865,7 @@
         <v>1604</v>
       </c>
       <c r="E165" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F165" t="s">
         <v>1605</v>
@@ -18909,7 +18930,7 @@
         <v>1613</v>
       </c>
       <c r="E166" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F166" t="s">
         <v>1614</v>
@@ -18974,7 +18995,7 @@
         <v>1623</v>
       </c>
       <c r="E167" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F167" t="s">
         <v>1624</v>
@@ -19039,7 +19060,7 @@
         <v>1633</v>
       </c>
       <c r="E168" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F168" t="s">
         <v>1634</v>
@@ -19104,7 +19125,7 @@
         <v>1643</v>
       </c>
       <c r="E169" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F169" t="s">
         <v>1636</v>
@@ -19163,7 +19184,7 @@
         <v>1653</v>
       </c>
       <c r="E170" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F170" t="s">
         <v>1654</v>
@@ -19228,7 +19249,7 @@
         <v>1662</v>
       </c>
       <c r="E171" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F171" t="s">
         <v>1663</v>
@@ -19293,7 +19314,7 @@
         <v>1672</v>
       </c>
       <c r="E172" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F172" t="s">
         <v>1673</v>
@@ -19358,7 +19379,7 @@
         <v>1683</v>
       </c>
       <c r="E173" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F173" t="s">
         <v>1684</v>
@@ -19423,7 +19444,7 @@
         <v>1693</v>
       </c>
       <c r="E174" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F174" t="s">
         <v>1694</v>
@@ -19488,7 +19509,7 @@
         <v>1705</v>
       </c>
       <c r="E175" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F175" t="s">
         <v>1706</v>
@@ -19550,7 +19571,7 @@
         <v>1715</v>
       </c>
       <c r="E176" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F176" t="s">
         <v>1716</v>
@@ -19615,7 +19636,7 @@
         <v>1724</v>
       </c>
       <c r="E177" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F177" t="s">
         <v>1708</v>
@@ -19680,7 +19701,7 @@
         <v>1733</v>
       </c>
       <c r="E178" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F178" t="s">
         <v>1686</v>
@@ -19745,7 +19766,7 @@
         <v>1741</v>
       </c>
       <c r="E179" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F179" t="s">
         <v>1742</v>
@@ -19810,7 +19831,7 @@
         <v>1751</v>
       </c>
       <c r="E180" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F180" t="s">
         <v>1752</v>
@@ -19875,7 +19896,7 @@
         <v>1762</v>
       </c>
       <c r="E181" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F181" t="s">
         <v>372</v>
@@ -19940,7 +19961,7 @@
         <v>1771</v>
       </c>
       <c r="E182" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F182" t="s">
         <v>1772</v>
@@ -20005,7 +20026,7 @@
         <v>1780</v>
       </c>
       <c r="E183" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F183" t="s">
         <v>1781</v>
@@ -20070,7 +20091,7 @@
         <v>1787</v>
       </c>
       <c r="E184" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F184" t="s">
         <v>1788</v>
@@ -20135,7 +20156,7 @@
         <v>1799</v>
       </c>
       <c r="E185" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F185" t="s">
         <v>1800</v>
@@ -20200,7 +20221,7 @@
         <v>1806</v>
       </c>
       <c r="E186" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F186" t="s">
         <v>111</v>
@@ -20265,7 +20286,7 @@
         <v>1817</v>
       </c>
       <c r="E187" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F187" t="s">
         <v>1818</v>
@@ -20330,7 +20351,7 @@
         <v>1826</v>
       </c>
       <c r="E188" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F188" t="s">
         <v>1764</v>
@@ -20395,7 +20416,7 @@
         <v>1836</v>
       </c>
       <c r="E189" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F189" t="s">
         <v>1837</v>
@@ -20460,7 +20481,7 @@
         <v>1848</v>
       </c>
       <c r="E190" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F190" t="s">
         <v>1849</v>
@@ -20525,7 +20546,7 @@
         <v>1858</v>
       </c>
       <c r="E191" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F191" t="s">
         <v>1820</v>
@@ -20590,7 +20611,7 @@
         <v>1869</v>
       </c>
       <c r="E192" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F192" t="s">
         <v>1870</v>
@@ -20646,7 +20667,7 @@
         <v>1879</v>
       </c>
       <c r="E193" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F193" t="s">
         <v>1880</v>
@@ -20711,7 +20732,7 @@
         <v>1888</v>
       </c>
       <c r="E194" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F194" t="s">
         <v>1889</v>
@@ -20776,7 +20797,7 @@
         <v>1897</v>
       </c>
       <c r="E195" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F195" t="s">
         <v>1898</v>
@@ -20841,7 +20862,7 @@
         <v>1910</v>
       </c>
       <c r="E196" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F196" t="s">
         <v>1900</v>
@@ -20906,7 +20927,7 @@
         <v>1919</v>
       </c>
       <c r="E197" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F197" t="s">
         <v>1920</v>
@@ -20965,7 +20986,7 @@
         <v>1928</v>
       </c>
       <c r="E198" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F198" t="s">
         <v>1929</v>
@@ -21012,7 +21033,7 @@
         <v>1936</v>
       </c>
       <c r="E199" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F199" t="s">
         <v>1150</v>
@@ -21077,7 +21098,7 @@
         <v>1945</v>
       </c>
       <c r="E200" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F200" t="s">
         <v>1946</v>
@@ -21130,7 +21151,7 @@
         <v>1954</v>
       </c>
       <c r="E201" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F201" t="s">
         <v>680</v>
@@ -21195,7 +21216,7 @@
         <v>1961</v>
       </c>
       <c r="E202" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F202" t="s">
         <v>1962</v>
@@ -21260,7 +21281,7 @@
         <v>1973</v>
       </c>
       <c r="E203" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F203" t="s">
         <v>281</v>
@@ -21316,7 +21337,7 @@
         <v>1980</v>
       </c>
       <c r="E204" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F204" t="s">
         <v>1981</v>
@@ -21381,7 +21402,7 @@
         <v>1993</v>
       </c>
       <c r="E205" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F205" t="s">
         <v>1141</v>
@@ -21446,7 +21467,7 @@
         <v>2003</v>
       </c>
       <c r="E206" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F206" t="s">
         <v>2004</v>
@@ -21511,7 +21532,7 @@
         <v>2014</v>
       </c>
       <c r="E207" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F207" t="s">
         <v>892</v>
@@ -21567,7 +21588,7 @@
         <v>2020</v>
       </c>
       <c r="E208" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F208" t="s">
         <v>1656</v>
@@ -21632,7 +21653,7 @@
         <v>2028</v>
       </c>
       <c r="E209" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F209" t="s">
         <v>2029</v>
@@ -21697,7 +21718,7 @@
         <v>2038</v>
       </c>
       <c r="E210" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F210" t="s">
         <v>1808</v>
@@ -21762,7 +21783,7 @@
         <v>2048</v>
       </c>
       <c r="E211" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F211" t="s">
         <v>1860</v>
@@ -21827,7 +21848,7 @@
         <v>2059</v>
       </c>
       <c r="E212" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F212" t="s">
         <v>2060</v>
@@ -21886,7 +21907,7 @@
         <v>2068</v>
       </c>
       <c r="E213" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F213" t="s">
         <v>2062</v>
@@ -21951,7 +21972,7 @@
         <v>2078</v>
       </c>
       <c r="E214" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F214" t="s">
         <v>1841</v>
@@ -22016,7 +22037,7 @@
         <v>2088</v>
       </c>
       <c r="E215" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F215" t="s">
         <v>470</v>
@@ -22081,7 +22102,7 @@
         <v>2097</v>
       </c>
       <c r="E216" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F216" t="s">
         <v>1840</v>
@@ -22146,7 +22167,7 @@
         <v>2107</v>
       </c>
       <c r="E217" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F217" t="s">
         <v>2007</v>
@@ -22205,7 +22226,7 @@
         <v>2116</v>
       </c>
       <c r="E218" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F218" t="s">
         <v>2117</v>
@@ -22258,7 +22279,7 @@
         <v>2124</v>
       </c>
       <c r="E219" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F219" t="s">
         <v>2125</v>
@@ -22323,7 +22344,7 @@
         <v>2136</v>
       </c>
       <c r="E220" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F220" t="s">
         <v>2137</v>
@@ -22388,7 +22409,7 @@
         <v>2148</v>
       </c>
       <c r="E221" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F221" t="s">
         <v>2149</v>
@@ -22453,7 +22474,7 @@
         <v>2157</v>
       </c>
       <c r="E222" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F222" t="s">
         <v>2158</v>
@@ -22518,7 +22539,7 @@
         <v>2166</v>
       </c>
       <c r="E223" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F223" t="s">
         <v>2167</v>
@@ -22583,7 +22604,7 @@
         <v>2175</v>
       </c>
       <c r="E224" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F224" t="s">
         <v>2176</v>
@@ -22642,7 +22663,7 @@
         <v>2182</v>
       </c>
       <c r="E225" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F225" t="s">
         <v>2170</v>
@@ -22707,7 +22728,7 @@
         <v>2193</v>
       </c>
       <c r="E226" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F226" t="s">
         <v>2161</v>
@@ -22772,7 +22793,7 @@
         <v>2204</v>
       </c>
       <c r="E227" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F227" t="s">
         <v>2139</v>
@@ -22837,7 +22858,7 @@
         <v>2214</v>
       </c>
       <c r="E228" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F228" t="s">
         <v>2215</v>
@@ -22902,7 +22923,7 @@
         <v>2225</v>
       </c>
       <c r="E229" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F229" t="s">
         <v>2160</v>
@@ -22967,7 +22988,7 @@
         <v>2236</v>
       </c>
       <c r="E230" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F230" t="s">
         <v>2237</v>
@@ -23032,7 +23053,7 @@
         <v>2245</v>
       </c>
       <c r="E231" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F231" t="s">
         <v>2246</v>
@@ -23091,7 +23112,7 @@
         <v>2252</v>
       </c>
       <c r="E232" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F232" t="s">
         <v>2253</v>
@@ -23129,7 +23150,7 @@
         <v>2261</v>
       </c>
       <c r="E233" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F233" t="s">
         <v>333</v>
@@ -23194,10 +23215,10 @@
         <v>2272</v>
       </c>
       <c r="D234" t="s">
-        <v>2478</v>
+        <v>2477</v>
       </c>
       <c r="E234" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F234" t="s">
         <v>807</v>
@@ -23262,10 +23283,10 @@
         <v>2281</v>
       </c>
       <c r="D235" t="s">
-        <v>2477</v>
+        <v>2476</v>
       </c>
       <c r="E235" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F235" t="s">
         <v>2279</v>
@@ -23330,7 +23351,7 @@
         <v>2287</v>
       </c>
       <c r="E236" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F236" t="s">
         <v>2288</v>
@@ -23395,7 +23416,7 @@
         <v>2296</v>
       </c>
       <c r="E237" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F237" t="s">
         <v>2297</v>
@@ -23460,7 +23481,7 @@
         <v>2307</v>
       </c>
       <c r="E238" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F238" t="s">
         <v>2308</v>
@@ -23525,7 +23546,7 @@
         <v>2317</v>
       </c>
       <c r="E239" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F239" t="s">
         <v>2318</v>
@@ -23590,7 +23611,7 @@
         <v>2328</v>
       </c>
       <c r="E240" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F240" t="s">
         <v>2329</v>
@@ -23655,7 +23676,7 @@
         <v>2337</v>
       </c>
       <c r="E241" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F241" t="s">
         <v>2338</v>
@@ -23720,7 +23741,7 @@
         <v>2350</v>
       </c>
       <c r="E242" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F242" t="s">
         <v>2351</v>
@@ -23782,7 +23803,7 @@
         <v>2360</v>
       </c>
       <c r="E243" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F243" t="s">
         <v>2361</v>
@@ -23847,7 +23868,7 @@
         <v>2371</v>
       </c>
       <c r="E244" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F244" t="s">
         <v>2363</v>
@@ -23912,7 +23933,7 @@
         <v>2383</v>
       </c>
       <c r="E245" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F245" t="s">
         <v>2384</v>
@@ -23977,7 +23998,7 @@
         <v>2392</v>
       </c>
       <c r="E246" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F246" t="s">
         <v>2393</v>
@@ -24039,7 +24060,7 @@
         <v>2402</v>
       </c>
       <c r="E247" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F247" t="s">
         <v>2403</v>
@@ -24104,7 +24125,7 @@
         <v>2413</v>
       </c>
       <c r="E248" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F248" t="s">
         <v>1790</v>
@@ -24169,7 +24190,7 @@
         <v>2422</v>
       </c>
       <c r="E249" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F249" t="s">
         <v>2423</v>
@@ -24234,7 +24255,7 @@
         <v>2434</v>
       </c>
       <c r="E250" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F250" t="s">
         <v>2435</v>
@@ -24290,7 +24311,7 @@
         <v>2463</v>
       </c>
       <c r="E251" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F251" t="s">
         <v>2040</v>
@@ -24307,7 +24328,7 @@
         <v>2465</v>
       </c>
       <c r="E252" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F252" t="s">
         <v>557</v>
@@ -24324,7 +24345,7 @@
         <v>2468</v>
       </c>
       <c r="E253" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F253" t="s">
         <v>2466</v>
@@ -24344,7 +24365,7 @@
         <v>2471</v>
       </c>
       <c r="E254" t="s">
-        <v>2508</v>
+        <v>2507</v>
       </c>
       <c r="F254" t="s">
         <v>2473</v>
@@ -24355,99 +24376,99 @@
     </row>
     <row r="255" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
+        <v>2478</v>
+      </c>
+      <c r="E255" t="s">
+        <v>2504</v>
+      </c>
+      <c r="G255" t="s">
         <v>2479</v>
-      </c>
-      <c r="E255" t="s">
-        <v>2505</v>
-      </c>
-      <c r="G255" t="s">
-        <v>2480</v>
       </c>
     </row>
     <row r="256" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
-        <v>2481</v>
+        <v>2480</v>
       </c>
       <c r="E256" t="s">
-        <v>2505</v>
+        <v>2504</v>
       </c>
       <c r="G256" t="s">
-        <v>2486</v>
+        <v>2485</v>
       </c>
     </row>
     <row r="257" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
-        <v>2482</v>
+        <v>2481</v>
       </c>
       <c r="E257" t="s">
-        <v>2505</v>
+        <v>2504</v>
       </c>
       <c r="G257" t="s">
-        <v>2487</v>
+        <v>2486</v>
       </c>
     </row>
     <row r="258" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
-        <v>2483</v>
+        <v>2482</v>
       </c>
       <c r="E258" t="s">
-        <v>2505</v>
+        <v>2504</v>
       </c>
       <c r="G258" t="s">
-        <v>2488</v>
+        <v>2487</v>
       </c>
     </row>
     <row r="259" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
-        <v>2484</v>
+        <v>2483</v>
       </c>
       <c r="E259" t="s">
-        <v>2505</v>
+        <v>2504</v>
       </c>
       <c r="G259" t="s">
-        <v>2489</v>
+        <v>2488</v>
       </c>
     </row>
     <row r="260" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
-        <v>2495</v>
+        <v>2494</v>
       </c>
       <c r="E260" t="s">
-        <v>2505</v>
+        <v>2504</v>
       </c>
       <c r="G260" t="s">
-        <v>2509</v>
+        <v>2508</v>
       </c>
     </row>
     <row r="261" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
+        <v>2490</v>
+      </c>
+      <c r="C261" t="s">
         <v>2491</v>
       </c>
-      <c r="C261" t="s">
-        <v>2492</v>
-      </c>
       <c r="D261" t="s">
-        <v>2485</v>
+        <v>2484</v>
       </c>
       <c r="E261" t="s">
-        <v>2506</v>
+        <v>2505</v>
       </c>
       <c r="F261" t="s">
-        <v>2496</v>
+        <v>2495</v>
       </c>
       <c r="G261" t="s">
-        <v>2490</v>
+        <v>2489</v>
       </c>
     </row>
     <row r="262" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
+        <v>2509</v>
+      </c>
+      <c r="B262" t="s">
+        <v>2509</v>
+      </c>
+      <c r="D262" t="s">
         <v>2510</v>
-      </c>
-      <c r="B262" t="s">
-        <v>2510</v>
-      </c>
-      <c r="D262" t="s">
-        <v>2511</v>
       </c>
       <c r="G262" t="s">
         <v>1496</v>
@@ -24455,64 +24476,64 @@
     </row>
     <row r="263" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
-        <v>2493</v>
+        <v>2492</v>
       </c>
       <c r="E263" t="s">
-        <v>2507</v>
+        <v>2506</v>
       </c>
       <c r="F263" t="s">
         <v>20</v>
       </c>
       <c r="G263" t="s">
-        <v>2494</v>
+        <v>2493</v>
       </c>
     </row>
     <row r="264" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
-        <v>2497</v>
+        <v>2496</v>
       </c>
       <c r="E264" t="s">
-        <v>2507</v>
+        <v>2506</v>
       </c>
       <c r="F264" t="s">
         <v>605</v>
       </c>
       <c r="G264" t="s">
-        <v>2498</v>
+        <v>2497</v>
       </c>
     </row>
     <row r="265" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
+        <v>2498</v>
+      </c>
+      <c r="D265" t="s">
+        <v>2501</v>
+      </c>
+      <c r="E265" t="s">
+        <v>2505</v>
+      </c>
+      <c r="F265" t="s">
         <v>2499</v>
       </c>
-      <c r="D265" t="s">
-        <v>2502</v>
-      </c>
-      <c r="E265" t="s">
-        <v>2506</v>
-      </c>
-      <c r="F265" t="s">
+      <c r="G265" t="s">
         <v>2500</v>
-      </c>
-      <c r="G265" t="s">
-        <v>2501</v>
       </c>
     </row>
     <row r="266" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
+        <v>2511</v>
+      </c>
+      <c r="D266" t="s">
+        <v>2514</v>
+      </c>
+      <c r="E266" t="s">
+        <v>2513</v>
+      </c>
+      <c r="F266" t="s">
+        <v>2515</v>
+      </c>
+      <c r="G266" t="s">
         <v>2512</v>
-      </c>
-      <c r="D266" t="s">
-        <v>2515</v>
-      </c>
-      <c r="E266" t="s">
-        <v>2514</v>
-      </c>
-      <c r="F266" t="s">
-        <v>2516</v>
-      </c>
-      <c r="G266" t="s">
-        <v>2513</v>
       </c>
     </row>
   </sheetData>

</xml_diff>